<commit_message>
+ Suicide attempts in front of trains
</commit_message>
<xml_diff>
--- a/Business/1979-2020 spoordata.xlsx
+++ b/Business/1979-2020 spoordata.xlsx
@@ -5,22 +5,33 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weilin\Desktop\School\Proftaak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weilin\Desktop\School\Proftaak\proftaak22\Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E44AE93-F44C-4F22-BB7E-D8BA8DBD675A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98463B30-CB2D-41BC-A11C-C69615737873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="28145" windowHeight="17062" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overledenen__zelfdoding__inwone" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="8">
   <si>
     <t>Geslacht</t>
   </si>
@@ -41,6 +52,9 @@
   </si>
   <si>
     <t>DMV_trein</t>
+  </si>
+  <si>
+    <t>DMV_trein_attempts</t>
   </si>
 </sst>
 </file>
@@ -524,8 +538,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -881,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.3"/>
@@ -895,7 +910,7 @@
     <col min="4" max="4" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,8 +923,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -922,8 +940,12 @@
       <c r="D2">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <f>D2/90.9*100</f>
+        <v>132.013201320132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -936,8 +958,12 @@
       <c r="D3">
         <v>152</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E66" si="0">D3/90.9*100</f>
+        <v>167.21672167216721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -950,8 +976,12 @@
       <c r="D4">
         <v>146</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>160.6160616061606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -964,8 +994,12 @@
       <c r="D5">
         <v>160</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>176.01760176017601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -978,8 +1012,12 @@
       <c r="D6">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>210.12101210121011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -992,8 +1030,12 @@
       <c r="D7">
         <v>194</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>213.4213421342134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1006,8 +1048,12 @@
       <c r="D8">
         <v>182</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>200.22002200220021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1020,8 +1066,12 @@
       <c r="D9">
         <v>182</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>200.22002200220021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1034,8 +1084,12 @@
       <c r="D10">
         <v>189</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>207.92079207920793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1048,8 +1102,12 @@
       <c r="D11">
         <v>184</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>202.42024202420242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1062,8 +1120,12 @@
       <c r="D12">
         <v>222</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>244.22442244224419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1076,8 +1138,12 @@
       <c r="D13">
         <v>173</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>190.31903190319031</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1090,8 +1156,12 @@
       <c r="D14">
         <v>181</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>199.1199119911991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1104,8 +1174,12 @@
       <c r="D15">
         <v>227</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>249.72497249724972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1118,8 +1192,12 @@
       <c r="D16">
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>220.02200220021999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1132,8 +1210,12 @@
       <c r="D17">
         <v>212</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>233.22332233223321</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1146,8 +1228,12 @@
       <c r="D18">
         <v>186</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>204.62046204620461</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1160,8 +1246,12 @@
       <c r="D19">
         <v>160</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>176.01760176017601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1174,8 +1264,12 @@
       <c r="D20">
         <v>167</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>183.71837183718372</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1188,8 +1282,12 @@
       <c r="D21">
         <v>176</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>193.6193619361936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1202,8 +1300,12 @@
       <c r="D22">
         <v>164</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>180.4180418041804</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1216,8 +1318,12 @@
       <c r="D23">
         <v>178</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>195.81958195819581</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1230,8 +1336,12 @@
       <c r="D24">
         <v>189</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>207.92079207920793</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1244,8 +1354,12 @@
       <c r="D25">
         <v>168</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>184.8184818481848</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1258,8 +1372,12 @@
       <c r="D26">
         <v>163</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>179.3179317931793</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1272,8 +1390,12 @@
       <c r="D27">
         <v>163</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>179.3179317931793</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1286,8 +1408,12 @@
       <c r="D28">
         <v>177</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>194.71947194719471</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1300,8 +1426,12 @@
       <c r="D29">
         <v>178</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="1">
+        <f t="shared" si="0"/>
+        <v>195.81958195819581</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1314,8 +1444,12 @@
       <c r="D30">
         <v>188</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="1">
+        <f t="shared" si="0"/>
+        <v>206.82068206820679</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1328,8 +1462,12 @@
       <c r="D31">
         <v>156</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>171.61716171617161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1342,8 +1480,12 @@
       <c r="D32">
         <v>187</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="1">
+        <f t="shared" si="0"/>
+        <v>205.72057205720569</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1356,8 +1498,12 @@
       <c r="D33">
         <v>182</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="1">
+        <f t="shared" si="0"/>
+        <v>200.22002200220021</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1370,8 +1516,12 @@
       <c r="D34">
         <v>205</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="1">
+        <f t="shared" si="0"/>
+        <v>225.52255225522549</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1384,8 +1534,12 @@
       <c r="D35">
         <v>188</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="1">
+        <f t="shared" si="0"/>
+        <v>206.82068206820679</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1398,8 +1552,12 @@
       <c r="D36">
         <v>187</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36" s="1">
+        <f t="shared" si="0"/>
+        <v>205.72057205720569</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1412,8 +1570,12 @@
       <c r="D37">
         <v>181</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="1">
+        <f t="shared" si="0"/>
+        <v>199.1199119911991</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1426,8 +1588,12 @@
       <c r="D38">
         <v>207</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="1">
+        <f t="shared" si="0"/>
+        <v>227.7227722772277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1440,8 +1606,12 @@
       <c r="D39">
         <v>209</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39" s="1">
+        <f t="shared" si="0"/>
+        <v>229.92299229922989</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1454,8 +1624,12 @@
       <c r="D40">
         <v>213</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40" s="1">
+        <f t="shared" si="0"/>
+        <v>234.32343234323429</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1468,8 +1642,12 @@
       <c r="D41">
         <v>186</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" s="1">
+        <f t="shared" si="0"/>
+        <v>204.62046204620461</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1482,8 +1660,12 @@
       <c r="D42">
         <v>188</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42" s="1">
+        <f t="shared" si="0"/>
+        <v>206.82068206820679</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1496,8 +1678,12 @@
       <c r="D43">
         <v>180</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43" s="1">
+        <f t="shared" si="0"/>
+        <v>198.01980198019803</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1510,8 +1696,12 @@
       <c r="D44">
         <v>67</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44" s="1">
+        <f t="shared" si="0"/>
+        <v>73.707370737073703</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -1524,8 +1714,12 @@
       <c r="D45">
         <v>92</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="1">
+        <f t="shared" si="0"/>
+        <v>101.21012101210121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -1538,8 +1732,12 @@
       <c r="D46">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="1">
+        <f t="shared" si="0"/>
+        <v>100.1100110011001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -1552,8 +1750,12 @@
       <c r="D47">
         <v>99</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47" s="1">
+        <f t="shared" si="0"/>
+        <v>108.9108910891089</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -1566,8 +1768,12 @@
       <c r="D48">
         <v>125</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48" s="1">
+        <f t="shared" si="0"/>
+        <v>137.5137513751375</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -1580,8 +1786,12 @@
       <c r="D49">
         <v>111</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49" s="1">
+        <f t="shared" si="0"/>
+        <v>122.1122112211221</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -1594,8 +1804,12 @@
       <c r="D50">
         <v>118</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50" s="1">
+        <f t="shared" si="0"/>
+        <v>129.81298129812981</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -1608,8 +1822,12 @@
       <c r="D51">
         <v>108</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="1">
+        <f t="shared" si="0"/>
+        <v>118.8118811881188</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -1622,8 +1840,12 @@
       <c r="D52">
         <v>115</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52" s="1">
+        <f t="shared" si="0"/>
+        <v>126.51265126512649</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -1636,8 +1858,12 @@
       <c r="D53">
         <v>119</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53" s="1">
+        <f t="shared" si="0"/>
+        <v>130.91309130913092</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -1650,8 +1876,12 @@
       <c r="D54">
         <v>131</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54" s="1">
+        <f t="shared" si="0"/>
+        <v>144.11441144114409</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1664,8 +1894,12 @@
       <c r="D55">
         <v>111</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55" s="1">
+        <f t="shared" si="0"/>
+        <v>122.1122112211221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -1678,8 +1912,12 @@
       <c r="D56">
         <v>110</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56" s="1">
+        <f t="shared" si="0"/>
+        <v>121.012101210121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -1692,8 +1930,12 @@
       <c r="D57">
         <v>146</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57" s="1">
+        <f t="shared" si="0"/>
+        <v>160.6160616061606</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -1706,8 +1948,12 @@
       <c r="D58">
         <v>140</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58" s="1">
+        <f t="shared" si="0"/>
+        <v>154.01540154015402</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -1720,8 +1966,12 @@
       <c r="D59">
         <v>139</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59" s="1">
+        <f t="shared" si="0"/>
+        <v>152.91529152915291</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -1734,8 +1984,12 @@
       <c r="D60">
         <v>118</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60" s="1">
+        <f t="shared" si="0"/>
+        <v>129.81298129812981</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -1748,8 +2002,12 @@
       <c r="D61">
         <v>111</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61" s="1">
+        <f t="shared" si="0"/>
+        <v>122.1122112211221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -1762,8 +2020,12 @@
       <c r="D62">
         <v>112</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62" s="1">
+        <f t="shared" si="0"/>
+        <v>123.2123212321232</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -1776,8 +2038,12 @@
       <c r="D63">
         <v>117</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63" s="1">
+        <f t="shared" si="0"/>
+        <v>128.71287128712871</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -1790,8 +2056,12 @@
       <c r="D64">
         <v>115</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64" s="1">
+        <f t="shared" si="0"/>
+        <v>126.51265126512649</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -1804,8 +2074,12 @@
       <c r="D65">
         <v>115</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E65" s="1">
+        <f t="shared" si="0"/>
+        <v>126.51265126512649</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -1818,8 +2092,12 @@
       <c r="D66">
         <v>126</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E66" s="1">
+        <f t="shared" si="0"/>
+        <v>138.61386138613861</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -1832,8 +2110,12 @@
       <c r="D67">
         <v>114</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E67" s="1">
+        <f t="shared" ref="E67:E127" si="1">D67/90.9*100</f>
+        <v>125.4125412541254</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -1846,8 +2128,12 @@
       <c r="D68">
         <v>104</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E68" s="1">
+        <f t="shared" si="1"/>
+        <v>114.41144114411441</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -1860,8 +2146,12 @@
       <c r="D69">
         <v>112</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E69" s="1">
+        <f t="shared" si="1"/>
+        <v>123.2123212321232</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -1874,8 +2164,12 @@
       <c r="D70">
         <v>127</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E70" s="1">
+        <f t="shared" si="1"/>
+        <v>139.71397139713972</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -1888,8 +2182,12 @@
       <c r="D71">
         <v>117</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E71" s="1">
+        <f t="shared" si="1"/>
+        <v>128.71287128712871</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -1902,8 +2200,12 @@
       <c r="D72">
         <v>143</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E72" s="1">
+        <f t="shared" si="1"/>
+        <v>157.31573157315731</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -1916,8 +2218,12 @@
       <c r="D73">
         <v>99</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E73" s="1">
+        <f t="shared" si="1"/>
+        <v>108.9108910891089</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -1930,8 +2236,12 @@
       <c r="D74">
         <v>139</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E74" s="1">
+        <f t="shared" si="1"/>
+        <v>152.91529152915291</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -1944,8 +2254,12 @@
       <c r="D75">
         <v>129</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E75" s="1">
+        <f t="shared" si="1"/>
+        <v>141.9141914191419</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -1958,8 +2272,12 @@
       <c r="D76">
         <v>151</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E76" s="1">
+        <f t="shared" si="1"/>
+        <v>166.1166116611661</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -1972,8 +2290,12 @@
       <c r="D77">
         <v>129</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E77" s="1">
+        <f t="shared" si="1"/>
+        <v>141.9141914191419</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -1986,8 +2308,12 @@
       <c r="D78">
         <v>125</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E78" s="1">
+        <f t="shared" si="1"/>
+        <v>137.5137513751375</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -2000,8 +2326,12 @@
       <c r="D79">
         <v>128</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E79" s="1">
+        <f t="shared" si="1"/>
+        <v>140.81408140814079</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -2014,8 +2344,12 @@
       <c r="D80">
         <v>144</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E80" s="1">
+        <f t="shared" si="1"/>
+        <v>158.41584158415841</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -2028,8 +2362,12 @@
       <c r="D81">
         <v>140</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E81" s="1">
+        <f t="shared" si="1"/>
+        <v>154.01540154015402</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -2042,8 +2380,12 @@
       <c r="D82">
         <v>142</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E82" s="1">
+        <f t="shared" si="1"/>
+        <v>156.2156215621562</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -2056,8 +2398,12 @@
       <c r="D83">
         <v>119</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E83" s="1">
+        <f t="shared" si="1"/>
+        <v>130.91309130913092</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -2070,8 +2416,12 @@
       <c r="D84">
         <v>129</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E84" s="1">
+        <f t="shared" si="1"/>
+        <v>141.9141914191419</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -2084,8 +2434,12 @@
       <c r="D85">
         <v>131</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E85" s="1">
+        <f t="shared" si="1"/>
+        <v>144.11441144114409</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -2098,8 +2452,12 @@
       <c r="D86">
         <v>53</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E86" s="1">
+        <f t="shared" si="1"/>
+        <v>58.305830583058302</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>3</v>
       </c>
@@ -2112,8 +2470,12 @@
       <c r="D87">
         <v>60</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E87" s="1">
+        <f t="shared" si="1"/>
+        <v>66.006600660065999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -2126,8 +2488,12 @@
       <c r="D88">
         <v>55</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E88" s="1">
+        <f t="shared" si="1"/>
+        <v>60.506050605060501</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -2140,8 +2506,12 @@
       <c r="D89">
         <v>61</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E89" s="1">
+        <f t="shared" si="1"/>
+        <v>67.106710671067106</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -2154,8 +2524,12 @@
       <c r="D90">
         <v>66</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E90" s="1">
+        <f t="shared" si="1"/>
+        <v>72.607260726072596</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -2168,8 +2542,12 @@
       <c r="D91">
         <v>83</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E91" s="1">
+        <f t="shared" si="1"/>
+        <v>91.309130913091309</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -2182,8 +2560,12 @@
       <c r="D92">
         <v>64</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E92" s="1">
+        <f t="shared" si="1"/>
+        <v>70.407040704070397</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -2196,8 +2578,12 @@
       <c r="D93">
         <v>74</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E93" s="1">
+        <f t="shared" si="1"/>
+        <v>81.408140814081392</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -2210,8 +2596,12 @@
       <c r="D94">
         <v>74</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E94" s="1">
+        <f t="shared" si="1"/>
+        <v>81.408140814081392</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>3</v>
       </c>
@@ -2224,8 +2614,12 @@
       <c r="D95">
         <v>65</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E95" s="1">
+        <f t="shared" si="1"/>
+        <v>71.507150715071504</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>3</v>
       </c>
@@ -2238,8 +2632,12 @@
       <c r="D96">
         <v>91</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E96" s="1">
+        <f t="shared" si="1"/>
+        <v>100.1100110011001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -2252,8 +2650,12 @@
       <c r="D97">
         <v>62</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E97" s="1">
+        <f t="shared" si="1"/>
+        <v>68.206820682068198</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -2266,8 +2668,12 @@
       <c r="D98">
         <v>71</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E98" s="1">
+        <f t="shared" si="1"/>
+        <v>78.107810781078101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>3</v>
       </c>
@@ -2280,8 +2686,12 @@
       <c r="D99">
         <v>81</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E99" s="1">
+        <f t="shared" si="1"/>
+        <v>89.108910891089096</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>3</v>
       </c>
@@ -2294,8 +2704,12 @@
       <c r="D100">
         <v>60</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E100" s="1">
+        <f t="shared" si="1"/>
+        <v>66.006600660065999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>3</v>
       </c>
@@ -2308,8 +2722,12 @@
       <c r="D101">
         <v>73</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E101" s="1">
+        <f t="shared" si="1"/>
+        <v>80.3080308030803</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -2322,8 +2740,12 @@
       <c r="D102">
         <v>68</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E102" s="1">
+        <f t="shared" si="1"/>
+        <v>74.807480748074809</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>3</v>
       </c>
@@ -2336,8 +2758,12 @@
       <c r="D103">
         <v>49</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E103" s="1">
+        <f t="shared" si="1"/>
+        <v>53.905390539053897</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>3</v>
       </c>
@@ -2350,8 +2776,12 @@
       <c r="D104">
         <v>55</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E104" s="1">
+        <f t="shared" si="1"/>
+        <v>60.506050605060501</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>3</v>
       </c>
@@ -2364,8 +2794,12 @@
       <c r="D105">
         <v>59</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E105" s="1">
+        <f t="shared" si="1"/>
+        <v>64.906490649064907</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -2378,8 +2812,12 @@
       <c r="D106">
         <v>49</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E106" s="1">
+        <f t="shared" si="1"/>
+        <v>53.905390539053897</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -2392,8 +2830,12 @@
       <c r="D107">
         <v>63</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E107" s="1">
+        <f t="shared" si="1"/>
+        <v>69.306930693069305</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>3</v>
       </c>
@@ -2406,8 +2848,12 @@
       <c r="D108">
         <v>63</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E108" s="1">
+        <f t="shared" si="1"/>
+        <v>69.306930693069305</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -2420,8 +2866,12 @@
       <c r="D109">
         <v>54</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E109" s="1">
+        <f t="shared" si="1"/>
+        <v>59.405940594059402</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>3</v>
       </c>
@@ -2434,8 +2884,12 @@
       <c r="D110">
         <v>59</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E110" s="1">
+        <f t="shared" si="1"/>
+        <v>64.906490649064907</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>3</v>
       </c>
@@ -2448,8 +2902,12 @@
       <c r="D111">
         <v>51</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E111" s="1">
+        <f t="shared" si="1"/>
+        <v>56.10561056105611</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>3</v>
       </c>
@@ -2462,8 +2920,12 @@
       <c r="D112">
         <v>50</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E112" s="1">
+        <f t="shared" si="1"/>
+        <v>55.005500550054997</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>3</v>
       </c>
@@ -2476,8 +2938,12 @@
       <c r="D113">
         <v>61</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E113" s="1">
+        <f t="shared" si="1"/>
+        <v>67.106710671067106</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>3</v>
       </c>
@@ -2490,8 +2956,12 @@
       <c r="D114">
         <v>45</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E114" s="1">
+        <f t="shared" si="1"/>
+        <v>49.504950495049506</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>3</v>
       </c>
@@ -2504,8 +2974,12 @@
       <c r="D115">
         <v>57</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E115" s="1">
+        <f t="shared" si="1"/>
+        <v>62.7062706270627</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>3</v>
       </c>
@@ -2518,8 +2992,12 @@
       <c r="D116">
         <v>48</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E116" s="1">
+        <f t="shared" si="1"/>
+        <v>52.805280528052798</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>3</v>
       </c>
@@ -2532,8 +3010,12 @@
       <c r="D117">
         <v>53</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E117" s="1">
+        <f t="shared" si="1"/>
+        <v>58.305830583058302</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>3</v>
       </c>
@@ -2546,8 +3028,12 @@
       <c r="D118">
         <v>54</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E118" s="1">
+        <f t="shared" si="1"/>
+        <v>59.405940594059402</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>3</v>
       </c>
@@ -2560,8 +3046,12 @@
       <c r="D119">
         <v>59</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E119" s="1">
+        <f t="shared" si="1"/>
+        <v>64.906490649064907</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>3</v>
       </c>
@@ -2574,8 +3064,12 @@
       <c r="D120">
         <v>62</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E120" s="1">
+        <f t="shared" si="1"/>
+        <v>68.206820682068198</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>3</v>
       </c>
@@ -2588,8 +3082,12 @@
       <c r="D121">
         <v>53</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E121" s="1">
+        <f t="shared" si="1"/>
+        <v>58.305830583058302</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -2602,8 +3100,12 @@
       <c r="D122">
         <v>63</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E122" s="1">
+        <f t="shared" si="1"/>
+        <v>69.306930693069305</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>3</v>
       </c>
@@ -2616,8 +3118,12 @@
       <c r="D123">
         <v>69</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E123" s="1">
+        <f t="shared" si="1"/>
+        <v>75.907590759075902</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>3</v>
       </c>
@@ -2630,8 +3136,12 @@
       <c r="D124">
         <v>71</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E124" s="1">
+        <f t="shared" si="1"/>
+        <v>78.107810781078101</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -2644,8 +3154,12 @@
       <c r="D125">
         <v>67</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E125" s="1">
+        <f t="shared" si="1"/>
+        <v>73.707370737073703</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -2658,8 +3172,12 @@
       <c r="D126">
         <v>59</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E126" s="1">
+        <f t="shared" si="1"/>
+        <v>64.906490649064907</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -2672,8 +3190,13 @@
       <c r="D127">
         <v>49</v>
       </c>
+      <c r="E127" s="1">
+        <f t="shared" si="1"/>
+        <v>53.905390539053897</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Spoordata predictions+solution Aanrijding Storingen
</commit_message>
<xml_diff>
--- a/Business/1979-2020 spoordata.xlsx
+++ b/Business/1979-2020 spoordata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weilin\Desktop\School\Proftaak\proftaak22\Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98463B30-CB2D-41BC-A11C-C69615737873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CD6CFF-A623-40E8-87B2-1B29695D26E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="28145" windowHeight="17062" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -899,7 +899,7 @@
   <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F10" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.3"/>

</xml_diff>